<commit_message>
feat: upload excel untuk jurnal manual (60%)
</commit_message>
<xml_diff>
--- a/public/vendor/js-xlsx/template-journal-excel.xlsx
+++ b/public/vendor/js-xlsx/template-journal-excel.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,24 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Akun Debet (L/R)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Akun Kredit (NRC)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKUN DEBET (L/R)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKUN KREDIT (NRC)</t>
   </si>
   <si>
     <t xml:space="preserve">KODE DEPO</t>
   </si>
   <si>
-    <t xml:space="preserve">NIK/FAKTUR</t>
+    <t xml:space="preserve">REFERENSI</t>
   </si>
   <si>
     <t xml:space="preserve">DESKRIPSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANGGAL</t>
   </si>
   <si>
     <t xml:space="preserve">JUMLAH</t>
@@ -113,15 +116,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -173,14 +178,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -257,14 +254,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,6 +283,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,11 +299,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,7 +311,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,7 +329,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal 2 2" xfId="20"/>
     <cellStyle name="Normal 6" xfId="21"/>
-    <cellStyle name="Excel Built-in Comma [0]" xfId="22"/>
+    <cellStyle name="Excel Built-in Comma [0] 1" xfId="22"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -392,296 +399,333 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="15.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C2" s="6" t="n">
+      <c r="B2" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>211013</v>
       </c>
-      <c r="D2" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>3156478.95</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>211013</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H3" s="11" t="n">
+        <v>3156478.95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>211013</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>3156478.95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>211013</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H5" s="11" t="n">
+        <v>3156478.95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H6" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="B8" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H8" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="9" t="n">
-        <v>3156478.95</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>211013</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="B9" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="B10" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H10" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="G3" s="9" t="n">
-        <v>3156478.95</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>211013</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="B11" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>211014</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H11" s="13" t="n">
+        <v>3650916.15025</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9" t="n">
-        <v>3156478.95</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>211013</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="9" t="n">
-        <v>3156478.95</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C6" s="6" t="n">
+      <c r="B12" s="8" t="n">
+        <v>824033</v>
+      </c>
+      <c r="C12" s="8" t="n">
         <v>211014</v>
       </c>
-      <c r="D6" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D9" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="11" t="n">
-        <v>3650916.15025</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>824033</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>211014</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>555</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="11" t="n">
+      <c r="F12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <v>44501</v>
+      </c>
+      <c r="H12" s="13" t="n">
         <v>3650916.15025</v>
       </c>
     </row>

</xml_diff>